<commit_message>
actualização do planeamento de tarefas.xlsx
</commit_message>
<xml_diff>
--- a/Documentacao/planeamento de tarefas.xlsx
+++ b/Documentacao/planeamento de tarefas.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe\Documents\isep\LAPR5\TheLegend_2\Documentacao\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="5190"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
   <si>
     <t>Divisão de Tarefas</t>
   </si>
@@ -69,15 +74,6 @@
     <t>Billboards Estado Humor</t>
   </si>
   <si>
-    <t>Minijogo 1</t>
-  </si>
-  <si>
-    <t>Minijogo 2</t>
-  </si>
-  <si>
-    <t>Minijogo 3</t>
-  </si>
-  <si>
     <t>Val: Tooltip</t>
   </si>
   <si>
@@ -187,13 +183,22 @@
   </si>
   <si>
     <t>Filipe</t>
+  </si>
+  <si>
+    <t>Minijogo 1 - jogo do galo</t>
+  </si>
+  <si>
+    <t>Minijogo 2 - enforcado</t>
+  </si>
+  <si>
+    <t>Minijogo 3 - labirinto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,6 +777,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -817,43 +848,25 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -895,7 +908,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -927,9 +940,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -961,6 +975,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1136,14 +1151,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.140625" style="23" customWidth="1"/>
     <col min="2" max="2" width="56.7109375" customWidth="1"/>
@@ -1151,64 +1166,64 @@
     <col min="9" max="9" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A3" s="30" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="30" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="43" t="s">
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="58" t="s">
+      <c r="G4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="31"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="24" t="s">
+      <c r="H4" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -1219,11 +1234,15 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="40"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="25"/>
+      <c r="H5" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="45"/>
       <c r="B6" s="16" t="s">
         <v>11</v>
       </c>
@@ -1232,11 +1251,15 @@
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="41"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="25"/>
+      <c r="H6" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
@@ -1245,11 +1268,11 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="13"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="41"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="25"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="26"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="45"/>
       <c r="B8" s="16" t="s">
         <v>13</v>
       </c>
@@ -1258,11 +1281,15 @@
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="41"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="25"/>
+      <c r="H8" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
       <c r="B9" s="16" t="s">
         <v>14</v>
       </c>
@@ -1271,11 +1298,11 @@
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="41"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="25"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="26"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="45"/>
       <c r="B10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1284,11 +1311,11 @@
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="41"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="25"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="26"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="45"/>
       <c r="B11" s="16" t="s">
         <v>16</v>
       </c>
@@ -1297,554 +1324,556 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="13"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="41"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="25"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="26"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="45"/>
       <c r="B12" s="16" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="41"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="25"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="45"/>
       <c r="B13" s="16" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="41"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="25"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="26"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="45"/>
       <c r="B14" s="16" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="41"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="25"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="26"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="45"/>
       <c r="B15" s="16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="13"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="41"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="25"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="26"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="45"/>
       <c r="B16" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="41"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="25"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="26"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="45"/>
       <c r="B17" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="41"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A18" s="26"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="26"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="46"/>
       <c r="B18" s="17"/>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="14"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="42"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="24" t="s">
-        <v>43</v>
+      <c r="H18" s="42"/>
+      <c r="I18" s="27"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
+        <v>40</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="12"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="40"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="25"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="25"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="45"/>
       <c r="B20" s="16" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="41"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="25"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="45"/>
       <c r="B21" s="16" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="41"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="25"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="26"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="45"/>
       <c r="B22" s="16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G22" s="13"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="25"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="45"/>
       <c r="B23" s="16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="13"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="41"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="25"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="26"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="45"/>
       <c r="B24" s="16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="41"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="25"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="26"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="45"/>
       <c r="B25" s="16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="13"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="41"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A26" s="26"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="26"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="46"/>
       <c r="B26" s="17"/>
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="14"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="42"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="38" t="s">
-        <v>45</v>
+      <c r="H26" s="42"/>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="58" t="s">
+        <v>42</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H27" s="55"/>
-      <c r="I27" s="40" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="H27" s="40"/>
+      <c r="I27" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="48"/>
       <c r="B28" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H28" s="56"/>
-      <c r="I28" s="41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="H28" s="41"/>
+      <c r="I28" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="48"/>
       <c r="B29" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="13"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="41"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="28"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="26"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="48"/>
       <c r="B30" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="13"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="41"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="28"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="26"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="48"/>
       <c r="B31" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H31" s="56"/>
-      <c r="I31" s="41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="28"/>
+        <v>43</v>
+      </c>
+      <c r="H31" s="41"/>
+      <c r="I31" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="48"/>
       <c r="B32" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
       <c r="G32" s="13"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="41"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="28"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="26"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="48"/>
       <c r="B33" s="16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="13"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="41"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="28"/>
+      <c r="H33" s="41"/>
+      <c r="I33" s="26"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="48"/>
       <c r="B34" s="16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="13"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="41"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="28"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="26"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="48"/>
       <c r="B35" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="13"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="41"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="28"/>
+      <c r="H35" s="41"/>
+      <c r="I35" s="26"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="48"/>
       <c r="B36" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="13"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="41"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="28"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="26"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="48"/>
       <c r="B37" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="13"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="41"/>
-    </row>
-    <row r="38" spans="1:9" s="2" customFormat="1">
-      <c r="A38" s="28"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="26"/>
+    </row>
+    <row r="38" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="48"/>
       <c r="B38" s="16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
       <c r="F38" s="19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G38" s="21"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A39" s="29"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="49"/>
       <c r="B39" s="20"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
       <c r="G39" s="14"/>
-      <c r="H39" s="57"/>
-      <c r="I39" s="42"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="49" t="s">
-        <v>38</v>
+      <c r="H39" s="42"/>
+      <c r="I39" s="27"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>35</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="40"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="25"/>
-      <c r="B41" s="50" t="s">
-        <v>39</v>
+      <c r="H40" s="40"/>
+      <c r="I40" s="25"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="45"/>
+      <c r="B41" s="35" t="s">
+        <v>36</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="41"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="25"/>
-      <c r="B42" s="50" t="s">
-        <v>40</v>
+      <c r="H41" s="41"/>
+      <c r="I41" s="26"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="45"/>
+      <c r="B42" s="35" t="s">
+        <v>37</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="11"/>
-      <c r="H42" s="56"/>
-      <c r="I42" s="41"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="25"/>
-      <c r="B43" s="50" t="s">
-        <v>41</v>
+      <c r="H42" s="41"/>
+      <c r="I42" s="26"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="45"/>
+      <c r="B43" s="35" t="s">
+        <v>38</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
-      <c r="H43" s="56"/>
-      <c r="I43" s="41"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="25"/>
-      <c r="B44" s="50" t="s">
-        <v>42</v>
+      <c r="H43" s="41"/>
+      <c r="I43" s="26"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="45"/>
+      <c r="B44" s="35" t="s">
+        <v>39</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="41"/>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A45" s="26"/>
-      <c r="B45" s="51"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="26"/>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="46"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
-      <c r="H45" s="57"/>
-      <c r="I45" s="42"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="27" t="s">
+      <c r="H45" s="42"/>
+      <c r="I45" s="27"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="44" t="s">
+      <c r="C46" s="37"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="G46" s="38"/>
+      <c r="H46" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="I46" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="52"/>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53" t="s">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="48"/>
+      <c r="B47" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="G46" s="53"/>
-      <c r="H46" s="54" t="s">
-        <v>46</v>
-      </c>
-      <c r="I46" s="40" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="A47" s="28"/>
-      <c r="B47" s="45" t="s">
-        <v>49</v>
-      </c>
       <c r="C47" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H47" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="I47" s="41" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" thickBot="1">
-      <c r="A48" s="29"/>
-      <c r="B48" s="46" t="s">
+        <v>43</v>
+      </c>
+      <c r="H47" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="I47" s="26" t="s">
         <v>50</v>
       </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="49"/>
+      <c r="B48" s="31" t="s">
+        <v>47</v>
+      </c>
       <c r="C48" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H48" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="I48" s="42" t="s">
-        <v>53</v>
+        <v>43</v>
+      </c>
+      <c r="H48" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="I48" s="27" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1866,24 +1895,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
actualizacao doc de planeamento
</commit_message>
<xml_diff>
--- a/Documentacao/planeamento de tarefas.xlsx
+++ b/Documentacao/planeamento de tarefas.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filipe\Documents\isep\LAPR5\TheLegend_2\Documentacao\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="5190"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>Divisão de Tarefas</t>
   </si>
@@ -197,8 +192,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -866,7 +861,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -908,7 +903,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -940,10 +935,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -975,7 +969,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1151,14 +1144,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="43.140625" style="23" customWidth="1"/>
     <col min="2" max="2" width="56.7109375" customWidth="1"/>
@@ -1166,7 +1159,7 @@
     <col min="9" max="9" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="27">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -1179,8 +1172,8 @@
       <c r="H1" s="53"/>
       <c r="I1" s="53"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1">
       <c r="A3" s="50" t="s">
         <v>1</v>
       </c>
@@ -1199,7 +1192,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" s="54"/>
       <c r="B4" s="54"/>
       <c r="C4" s="28" t="s">
@@ -1222,7 +1215,7 @@
       </c>
       <c r="I4" s="51"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="44" t="s">
         <v>9</v>
       </c>
@@ -1241,7 +1234,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="45"/>
       <c r="B6" s="16" t="s">
         <v>11</v>
@@ -1258,7 +1251,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="45"/>
       <c r="B7" s="16" t="s">
         <v>12</v>
@@ -1271,7 +1264,7 @@
       <c r="H7" s="41"/>
       <c r="I7" s="26"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="45"/>
       <c r="B8" s="16" t="s">
         <v>13</v>
@@ -1288,7 +1281,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="45"/>
       <c r="B9" s="16" t="s">
         <v>14</v>
@@ -1301,7 +1294,7 @@
       <c r="H9" s="41"/>
       <c r="I9" s="26"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="45"/>
       <c r="B10" s="16" t="s">
         <v>15</v>
@@ -1314,7 +1307,7 @@
       <c r="H10" s="41"/>
       <c r="I10" s="26"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="45"/>
       <c r="B11" s="16" t="s">
         <v>16</v>
@@ -1327,7 +1320,7 @@
       <c r="H11" s="41"/>
       <c r="I11" s="26"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="45"/>
       <c r="B12" s="16" t="s">
         <v>54</v>
@@ -1342,7 +1335,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="45"/>
       <c r="B13" s="16" t="s">
         <v>55</v>
@@ -1355,7 +1348,7 @@
       <c r="H13" s="41"/>
       <c r="I13" s="26"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="45"/>
       <c r="B14" s="16" t="s">
         <v>56</v>
@@ -1368,7 +1361,7 @@
       <c r="H14" s="41"/>
       <c r="I14" s="26"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="45"/>
       <c r="B15" s="16" t="s">
         <v>17</v>
@@ -1381,7 +1374,7 @@
       <c r="H15" s="41"/>
       <c r="I15" s="26"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="45"/>
       <c r="B16" s="16" t="s">
         <v>18</v>
@@ -1394,7 +1387,7 @@
       <c r="H16" s="41"/>
       <c r="I16" s="26"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" s="45"/>
       <c r="B17" s="16" t="s">
         <v>19</v>
@@ -1407,7 +1400,7 @@
       <c r="H17" s="41"/>
       <c r="I17" s="26"/>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15.75" thickBot="1">
       <c r="A18" s="46"/>
       <c r="B18" s="17"/>
       <c r="C18" s="8"/>
@@ -1418,7 +1411,7 @@
       <c r="H18" s="42"/>
       <c r="I18" s="27"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" s="44" t="s">
         <v>40</v>
       </c>
@@ -1433,7 +1426,7 @@
       <c r="H19" s="40"/>
       <c r="I19" s="25"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" s="45"/>
       <c r="B20" s="16" t="s">
         <v>55</v>
@@ -1446,7 +1439,7 @@
       <c r="H20" s="41"/>
       <c r="I20" s="26"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="45"/>
       <c r="B21" s="16" t="s">
         <v>56</v>
@@ -1459,7 +1452,7 @@
       <c r="H21" s="41"/>
       <c r="I21" s="26"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="45"/>
       <c r="B22" s="16" t="s">
         <v>20</v>
@@ -1478,20 +1471,24 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="45"/>
       <c r="B23" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="E23" s="11" t="s">
+        <v>43</v>
+      </c>
       <c r="F23" s="11"/>
       <c r="G23" s="13"/>
       <c r="H23" s="41"/>
-      <c r="I23" s="26"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="45"/>
       <c r="B24" s="16" t="s">
         <v>22</v>
@@ -1504,7 +1501,7 @@
       <c r="H24" s="41"/>
       <c r="I24" s="26"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" s="45"/>
       <c r="B25" s="16" t="s">
         <v>23</v>
@@ -1517,7 +1514,7 @@
       <c r="H25" s="41"/>
       <c r="I25" s="26"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15.75" thickBot="1">
       <c r="A26" s="46"/>
       <c r="B26" s="17"/>
       <c r="C26" s="8"/>
@@ -1528,7 +1525,7 @@
       <c r="H26" s="42"/>
       <c r="I26" s="27"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" s="58" t="s">
         <v>42</v>
       </c>
@@ -1551,7 +1548,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" s="48"/>
       <c r="B28" s="16" t="s">
         <v>25</v>
@@ -1570,7 +1567,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" s="48"/>
       <c r="B29" s="16" t="s">
         <v>26</v>
@@ -1583,7 +1580,7 @@
       <c r="H29" s="41"/>
       <c r="I29" s="26"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="A30" s="48"/>
       <c r="B30" s="16" t="s">
         <v>27</v>
@@ -1596,7 +1593,7 @@
       <c r="H30" s="41"/>
       <c r="I30" s="26"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9">
       <c r="A31" s="48"/>
       <c r="B31" s="16" t="s">
         <v>28</v>
@@ -1615,7 +1612,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9">
       <c r="A32" s="48"/>
       <c r="B32" s="16" t="s">
         <v>29</v>
@@ -1628,7 +1625,7 @@
       <c r="H32" s="41"/>
       <c r="I32" s="26"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9">
       <c r="A33" s="48"/>
       <c r="B33" s="16" t="s">
         <v>30</v>
@@ -1641,7 +1638,7 @@
       <c r="H33" s="41"/>
       <c r="I33" s="26"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="48"/>
       <c r="B34" s="16" t="s">
         <v>31</v>
@@ -1654,7 +1651,7 @@
       <c r="H34" s="41"/>
       <c r="I34" s="26"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9">
       <c r="A35" s="48"/>
       <c r="B35" s="16" t="s">
         <v>32</v>
@@ -1667,7 +1664,7 @@
       <c r="H35" s="41"/>
       <c r="I35" s="26"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
       <c r="A36" s="48"/>
       <c r="B36" s="16" t="s">
         <v>33</v>
@@ -1680,7 +1677,7 @@
       <c r="H36" s="41"/>
       <c r="I36" s="26"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9">
       <c r="A37" s="48"/>
       <c r="B37" s="16" t="s">
         <v>34</v>
@@ -1693,7 +1690,7 @@
       <c r="H37" s="41"/>
       <c r="I37" s="26"/>
     </row>
-    <row r="38" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="2" customFormat="1">
       <c r="A38" s="48"/>
       <c r="B38" s="16" t="s">
         <v>44</v>
@@ -1712,7 +1709,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15.75" thickBot="1">
       <c r="A39" s="49"/>
       <c r="B39" s="20"/>
       <c r="C39" s="8"/>
@@ -1723,7 +1720,7 @@
       <c r="H39" s="42"/>
       <c r="I39" s="27"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9">
       <c r="A40" s="44" t="s">
         <v>41</v>
       </c>
@@ -1738,7 +1735,7 @@
       <c r="H40" s="40"/>
       <c r="I40" s="25"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9">
       <c r="A41" s="45"/>
       <c r="B41" s="35" t="s">
         <v>36</v>
@@ -1751,7 +1748,7 @@
       <c r="H41" s="41"/>
       <c r="I41" s="26"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="45"/>
       <c r="B42" s="35" t="s">
         <v>37</v>
@@ -1764,7 +1761,7 @@
       <c r="H42" s="41"/>
       <c r="I42" s="26"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9">
       <c r="A43" s="45"/>
       <c r="B43" s="35" t="s">
         <v>38</v>
@@ -1777,7 +1774,7 @@
       <c r="H43" s="41"/>
       <c r="I43" s="26"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9">
       <c r="A44" s="45"/>
       <c r="B44" s="35" t="s">
         <v>39</v>
@@ -1790,7 +1787,7 @@
       <c r="H44" s="41"/>
       <c r="I44" s="26"/>
     </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15.75" thickBot="1">
       <c r="A45" s="46"/>
       <c r="B45" s="36"/>
       <c r="C45" s="8"/>
@@ -1801,7 +1798,7 @@
       <c r="H45" s="42"/>
       <c r="I45" s="27"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" s="47" t="s">
         <v>45</v>
       </c>
@@ -1822,7 +1819,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="48"/>
       <c r="B47" s="30" t="s">
         <v>46</v>
@@ -1849,7 +1846,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15.75" thickBot="1">
       <c r="A48" s="49"/>
       <c r="B48" s="31" t="s">
         <v>47</v>
@@ -1895,24 +1892,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Colocação dos Pedidos a funcionar, ainda faltam algumas validações, mas já dá para fazer testes.
Campo UserAsk é quem vai fazer a introdução, UserOrigin é quem fazem o pedido e o UserDestin é quem vai receber a introdução.
</commit_message>
<xml_diff>
--- a/Documentacao/planeamento de tarefas.xlsx
+++ b/Documentacao/planeamento de tarefas.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel Mendes\Desktop\TheLegend\Documentacao\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="5190"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
   <si>
     <t>Divisão de Tarefas</t>
   </si>
@@ -196,7 +201,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +219,13 @@
       <b/>
       <sz val="22"/>
       <color theme="6" tint="-0.499984740745262"/>
+      <name val="Century Schoolbook"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Century Schoolbook"/>
       <family val="1"/>
     </font>
@@ -750,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -846,6 +858,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -866,7 +879,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -904,9 +917,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -941,7 +954,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -976,7 +989,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1152,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,15 +1551,13 @@
       <c r="A27" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="59" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>43</v>
-      </c>
+      <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="12" t="s">
@@ -1565,9 +1576,7 @@
       <c r="C28" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>43</v>
-      </c>
+      <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="13" t="s">

</xml_diff>

<commit_message>
Actualização do planeamento de tarefas.
Web Site:
Melhoramentos na class Introdution, Pedidos já dão origem as Introduções.

Configurações necessarias para colocar o site online e a BD no serviços.
</commit_message>
<xml_diff>
--- a/Documentacao/planeamento de tarefas.xlsx
+++ b/Documentacao/planeamento de tarefas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel Mendes\Desktop\TheLegend\Documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\TheLegend\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
   <si>
     <t>Divisão de Tarefas</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Friend Requests</t>
-  </si>
-  <si>
     <t>Download</t>
   </si>
   <si>
@@ -195,13 +192,34 @@
   </si>
   <si>
     <t>Iniciado</t>
+  </si>
+  <si>
+    <t>Pedidos</t>
+  </si>
+  <si>
+    <t>Introduções</t>
+  </si>
+  <si>
+    <t>Humor</t>
+  </si>
+  <si>
+    <t>Estados</t>
+  </si>
+  <si>
+    <t>Jogos</t>
+  </si>
+  <si>
+    <t>Perfil</t>
+  </si>
+  <si>
+    <t>Missions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +247,14 @@
       <name val="Century Schoolbook"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -762,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -815,6 +841,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -855,10 +882,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1163,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,41 +1210,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="58"/>
       <c r="H3" s="24"/>
-      <c r="I3" s="50" t="s">
-        <v>49</v>
+      <c r="I3" s="51" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
+      <c r="A4" s="55"/>
+      <c r="B4" s="55"/>
       <c r="C4" s="28" t="s">
         <v>4</v>
       </c>
@@ -1229,12 +1261,12 @@
         <v>6</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" s="51"/>
+        <v>51</v>
+      </c>
+      <c r="I4" s="52"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="45" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -1246,14 +1278,14 @@
       <c r="F5" s="7"/>
       <c r="G5" s="12"/>
       <c r="H5" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I5" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="A6" s="46"/>
       <c r="B6" s="16" t="s">
         <v>11</v>
       </c>
@@ -1263,14 +1295,14 @@
       <c r="F6" s="11"/>
       <c r="G6" s="13"/>
       <c r="H6" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I6" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="A7" s="46"/>
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
@@ -1283,7 +1315,7 @@
       <c r="I7" s="26"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="A8" s="46"/>
       <c r="B8" s="16" t="s">
         <v>13</v>
       </c>
@@ -1293,14 +1325,14 @@
       <c r="F8" s="11"/>
       <c r="G8" s="13"/>
       <c r="H8" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+      <c r="A9" s="46"/>
       <c r="B9" s="16" t="s">
         <v>14</v>
       </c>
@@ -1313,7 +1345,7 @@
       <c r="I9" s="26"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+      <c r="A10" s="46"/>
       <c r="B10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1326,7 +1358,7 @@
       <c r="I10" s="26"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="16" t="s">
         <v>16</v>
       </c>
@@ -1339,9 +1371,9 @@
       <c r="I11" s="26"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="45"/>
+      <c r="A12" s="46"/>
       <c r="B12" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
@@ -1350,13 +1382,13 @@
       <c r="G12" s="13"/>
       <c r="H12" s="41"/>
       <c r="I12" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+      <c r="A13" s="46"/>
       <c r="B13" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
@@ -1367,9 +1399,9 @@
       <c r="I13" s="26"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
@@ -1380,7 +1412,7 @@
       <c r="I14" s="26"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+      <c r="A15" s="46"/>
       <c r="B15" s="16" t="s">
         <v>17</v>
       </c>
@@ -1393,7 +1425,7 @@
       <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+      <c r="A16" s="46"/>
       <c r="B16" s="16" t="s">
         <v>18</v>
       </c>
@@ -1406,7 +1438,7 @@
       <c r="I16" s="26"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="46"/>
       <c r="B17" s="16" t="s">
         <v>19</v>
       </c>
@@ -1419,7 +1451,7 @@
       <c r="I17" s="26"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="46"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="17"/>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
@@ -1430,11 +1462,11 @@
       <c r="I18" s="27"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
-        <v>40</v>
+      <c r="A19" s="45" t="s">
+        <v>39</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
@@ -1445,9 +1477,9 @@
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="11"/>
@@ -1458,9 +1490,9 @@
       <c r="I20" s="26"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
+      <c r="A21" s="46"/>
       <c r="B21" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="11"/>
@@ -1471,60 +1503,60 @@
       <c r="I21" s="26"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="46"/>
       <c r="B22" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="41"/>
       <c r="I22" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="46"/>
       <c r="B23" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="13"/>
       <c r="H23" s="41"/>
       <c r="I23" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+      <c r="A24" s="46"/>
       <c r="B24" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="13"/>
       <c r="H24" s="41"/>
       <c r="I24" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
+      <c r="A25" s="46"/>
       <c r="B25" s="16" t="s">
         <v>23</v>
       </c>
@@ -1537,7 +1569,7 @@
       <c r="I25" s="26"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="46"/>
+      <c r="A26" s="47"/>
       <c r="B26" s="17"/>
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
@@ -1548,158 +1580,182 @@
       <c r="I26" s="27"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="59" t="s">
+      <c r="A27" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="44" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H27" s="40"/>
       <c r="I27" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H28" s="41"/>
       <c r="I28" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="16" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H29" s="41"/>
       <c r="I29" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="60"/>
       <c r="B30" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="10"/>
+        <v>61</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
-      <c r="G30" s="13"/>
+      <c r="G30" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="H30" s="41"/>
-      <c r="I30" s="26"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
+      <c r="I30" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="60"/>
       <c r="B31" s="16" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H31" s="41"/>
       <c r="I31" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="60"/>
       <c r="B32" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="10"/>
+        <v>62</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
-      <c r="G32" s="13"/>
+      <c r="G32" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="H32" s="41"/>
-      <c r="I32" s="26"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
+      <c r="I32" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="60"/>
       <c r="B33" s="16" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H33" s="41"/>
       <c r="I33" s="26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="60"/>
       <c r="B34" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="10"/>
+        <v>59</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
-      <c r="G34" s="13"/>
+      <c r="G34" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="H34" s="41"/>
-      <c r="I34" s="26"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
+      <c r="I34" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="60"/>
       <c r="B35" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="10"/>
+        <v>58</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
-      <c r="G35" s="13"/>
+      <c r="G35" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="H35" s="41"/>
-      <c r="I35" s="26"/>
+      <c r="I35" s="26" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="48"/>
+      <c r="A36" s="60"/>
       <c r="B36" s="16" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
@@ -1710,203 +1766,293 @@
       <c r="I36" s="26"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="48"/>
+      <c r="A37" s="60"/>
       <c r="B37" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="10"/>
+        <v>27</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
-      <c r="G37" s="13"/>
+      <c r="G37" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="H37" s="41"/>
-      <c r="I37" s="26"/>
-    </row>
-    <row r="38" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="48"/>
+      <c r="I37" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="60"/>
       <c r="B38" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="G38" s="21"/>
+        <v>28</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="13"/>
       <c r="H38" s="41"/>
-      <c r="I38" s="26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="49"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="27"/>
+      <c r="I38" s="26"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="60"/>
+      <c r="B39" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" s="41"/>
+      <c r="I39" s="26" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="25"/>
+      <c r="A40" s="60"/>
+      <c r="B40" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="41"/>
+      <c r="I40" s="26"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="45"/>
-      <c r="B41" s="35" t="s">
-        <v>36</v>
+      <c r="A41" s="60"/>
+      <c r="B41" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
+      <c r="G41" s="13"/>
       <c r="H41" s="41"/>
       <c r="I41" s="26"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="45"/>
-      <c r="B42" s="35" t="s">
-        <v>37</v>
+      <c r="A42" s="60"/>
+      <c r="B42" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
+      <c r="G42" s="13"/>
       <c r="H42" s="41"/>
       <c r="I42" s="26"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="45"/>
-      <c r="B43" s="35" t="s">
-        <v>38</v>
+      <c r="A43" s="60"/>
+      <c r="B43" s="16" t="s">
+        <v>33</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
+      <c r="G43" s="13"/>
       <c r="H43" s="41"/>
       <c r="I43" s="26"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="45"/>
-      <c r="B44" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
+    <row r="44" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="60"/>
+      <c r="B44" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="G44" s="21"/>
       <c r="H44" s="41"/>
-      <c r="I44" s="26"/>
+      <c r="I44" s="26" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="46"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="61"/>
+      <c r="B45" s="20"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
+      <c r="G45" s="14"/>
       <c r="H45" s="42"/>
       <c r="I45" s="27"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="47" t="s">
+      <c r="A46" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="25"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="46"/>
+      <c r="B47" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="26"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="46"/>
+      <c r="B48" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="10"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="41"/>
+      <c r="I48" s="26"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="46"/>
+      <c r="B49" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="10"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="26"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="46"/>
+      <c r="B50" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="26"/>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="47"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="42"/>
+      <c r="I51" s="27"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="37"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="G52" s="38"/>
+      <c r="H52" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="I52" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="49"/>
+      <c r="B53" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="37"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="G46" s="38"/>
-      <c r="H46" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="I46" s="25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="48"/>
-      <c r="B47" s="30" t="s">
+      <c r="C53" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H53" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="I53" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="50"/>
+      <c r="B54" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H47" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="I47" s="26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="49"/>
-      <c r="B48" s="31" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H48" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="I48" s="27" t="s">
-        <v>50</v>
+      <c r="C54" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H54" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="I54" s="27" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A40:A45"/>
-    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A46:A51"/>
+    <mergeCell ref="A52:A54"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:A4"/>
@@ -1914,7 +2060,7 @@
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="A5:A18"/>
     <mergeCell ref="A19:A26"/>
-    <mergeCell ref="A27:A39"/>
+    <mergeCell ref="A27:A45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
conclusao de amigos em 3 grau e atualizacao de planeamento
</commit_message>
<xml_diff>
--- a/Documentacao/planeamento de tarefas.xlsx
+++ b/Documentacao/planeamento de tarefas.xlsx
@@ -877,6 +877,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -926,9 +929,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1235,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,41 +1248,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="58"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="61"/>
       <c r="H3" s="24"/>
-      <c r="I3" s="51" t="s">
+      <c r="I3" s="54" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="55"/>
-      <c r="B4" s="55"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="28" t="s">
         <v>4</v>
       </c>
@@ -1301,10 +1301,10 @@
       <c r="H4" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="52"/>
+      <c r="I4" s="55"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="48" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -1323,7 +1323,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="16" t="s">
         <v>11</v>
       </c>
@@ -1340,7 +1340,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
@@ -1353,7 +1353,7 @@
       <c r="I7" s="26"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="16" t="s">
         <v>13</v>
       </c>
@@ -1370,7 +1370,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="16" t="s">
         <v>14</v>
       </c>
@@ -1383,7 +1383,7 @@
       <c r="I9" s="26"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1396,7 +1396,7 @@
       <c r="I10" s="26"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="16" t="s">
         <v>16</v>
       </c>
@@ -1409,7 +1409,7 @@
       <c r="I11" s="26"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="16" t="s">
         <v>52</v>
       </c>
@@ -1424,7 +1424,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="16" t="s">
         <v>53</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="I13" s="26"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="46"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="16" t="s">
         <v>54</v>
       </c>
@@ -1450,7 +1450,7 @@
       <c r="I14" s="26"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="16" t="s">
         <v>17</v>
       </c>
@@ -1463,7 +1463,7 @@
       <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="16" t="s">
         <v>18</v>
       </c>
@@ -1476,7 +1476,7 @@
       <c r="I16" s="26"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="46"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="16" t="s">
         <v>19</v>
       </c>
@@ -1489,7 +1489,7 @@
       <c r="I17" s="26"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="47"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="17"/>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
@@ -1500,7 +1500,7 @@
       <c r="I18" s="27"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="48" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="15" t="s">
@@ -1515,7 +1515,7 @@
       <c r="I19" s="25"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="16" t="s">
         <v>53</v>
       </c>
@@ -1528,7 +1528,7 @@
       <c r="I20" s="26"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="46"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="16" t="s">
         <v>54</v>
       </c>
@@ -1541,7 +1541,7 @@
       <c r="I21" s="26"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="16" t="s">
         <v>20</v>
       </c>
@@ -1560,7 +1560,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="46"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="16" t="s">
         <v>21</v>
       </c>
@@ -1573,11 +1573,11 @@
       <c r="G23" s="13"/>
       <c r="H23" s="41"/>
       <c r="I23" s="26" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
+      <c r="A24" s="49"/>
       <c r="B24" s="16" t="s">
         <v>22</v>
       </c>
@@ -1594,7 +1594,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="46"/>
+      <c r="A25" s="49"/>
       <c r="B25" s="16" t="s">
         <v>23</v>
       </c>
@@ -1607,8 +1607,8 @@
       <c r="I25" s="26"/>
     </row>
     <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="62" t="s">
+      <c r="A26" s="49"/>
+      <c r="B26" s="45" t="s">
         <v>64</v>
       </c>
       <c r="C26" s="18"/>
@@ -1618,13 +1618,13 @@
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="21"/>
-      <c r="H26" s="63"/>
-      <c r="I26" s="64" t="s">
+      <c r="H26" s="46"/>
+      <c r="I26" s="47" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="47"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="17"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
@@ -1635,7 +1635,7 @@
       <c r="I27" s="27"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="59" t="s">
+      <c r="A28" s="62" t="s">
         <v>41</v>
       </c>
       <c r="B28" s="44" t="s">
@@ -1656,7 +1656,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="60"/>
+      <c r="A29" s="63"/>
       <c r="B29" s="16" t="s">
         <v>25</v>
       </c>
@@ -1675,7 +1675,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="60"/>
+      <c r="A30" s="63"/>
       <c r="B30" s="16" t="s">
         <v>57</v>
       </c>
@@ -1694,7 +1694,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="60"/>
+      <c r="A31" s="63"/>
       <c r="B31" s="16" t="s">
         <v>61</v>
       </c>
@@ -1713,7 +1713,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="60"/>
+      <c r="A32" s="63"/>
       <c r="B32" s="16" t="s">
         <v>63</v>
       </c>
@@ -1732,7 +1732,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="60"/>
+      <c r="A33" s="63"/>
       <c r="B33" s="16" t="s">
         <v>62</v>
       </c>
@@ -1751,7 +1751,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="60"/>
+      <c r="A34" s="63"/>
       <c r="B34" s="16" t="s">
         <v>60</v>
       </c>
@@ -1770,7 +1770,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="60"/>
+      <c r="A35" s="63"/>
       <c r="B35" s="16" t="s">
         <v>59</v>
       </c>
@@ -1789,7 +1789,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="60"/>
+      <c r="A36" s="63"/>
       <c r="B36" s="16" t="s">
         <v>58</v>
       </c>
@@ -1808,7 +1808,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="60"/>
+      <c r="A37" s="63"/>
       <c r="B37" s="16" t="s">
         <v>26</v>
       </c>
@@ -1821,7 +1821,7 @@
       <c r="I37" s="26"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="60"/>
+      <c r="A38" s="63"/>
       <c r="B38" s="16" t="s">
         <v>27</v>
       </c>
@@ -1840,7 +1840,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="60"/>
+      <c r="A39" s="63"/>
       <c r="B39" s="16" t="s">
         <v>28</v>
       </c>
@@ -1853,7 +1853,7 @@
       <c r="I39" s="26"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="60"/>
+      <c r="A40" s="63"/>
       <c r="B40" s="16" t="s">
         <v>29</v>
       </c>
@@ -1872,7 +1872,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="60"/>
+      <c r="A41" s="63"/>
       <c r="B41" s="16" t="s">
         <v>30</v>
       </c>
@@ -1885,7 +1885,7 @@
       <c r="I41" s="26"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="60"/>
+      <c r="A42" s="63"/>
       <c r="B42" s="16" t="s">
         <v>31</v>
       </c>
@@ -1898,7 +1898,7 @@
       <c r="I42" s="26"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="60"/>
+      <c r="A43" s="63"/>
       <c r="B43" s="16" t="s">
         <v>32</v>
       </c>
@@ -1911,7 +1911,7 @@
       <c r="I43" s="26"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="60"/>
+      <c r="A44" s="63"/>
       <c r="B44" s="16" t="s">
         <v>33</v>
       </c>
@@ -1924,7 +1924,7 @@
       <c r="I44" s="26"/>
     </row>
     <row r="45" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="60"/>
+      <c r="A45" s="63"/>
       <c r="B45" s="16" t="s">
         <v>43</v>
       </c>
@@ -1941,7 +1941,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="61"/>
+      <c r="A46" s="64"/>
       <c r="B46" s="20"/>
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
@@ -1952,7 +1952,7 @@
       <c r="I46" s="27"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="48" t="s">
         <v>40</v>
       </c>
       <c r="B47" s="34" t="s">
@@ -1967,7 +1967,7 @@
       <c r="I47" s="25"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="46"/>
+      <c r="A48" s="49"/>
       <c r="B48" s="35" t="s">
         <v>35</v>
       </c>
@@ -1980,7 +1980,7 @@
       <c r="I48" s="26"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="46"/>
+      <c r="A49" s="49"/>
       <c r="B49" s="35" t="s">
         <v>36</v>
       </c>
@@ -1993,7 +1993,7 @@
       <c r="I49" s="26"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="46"/>
+      <c r="A50" s="49"/>
       <c r="B50" s="35" t="s">
         <v>37</v>
       </c>
@@ -2006,7 +2006,7 @@
       <c r="I50" s="26"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="46"/>
+      <c r="A51" s="49"/>
       <c r="B51" s="35" t="s">
         <v>38</v>
       </c>
@@ -2019,7 +2019,7 @@
       <c r="I51" s="26"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="47"/>
+      <c r="A52" s="50"/>
       <c r="B52" s="36"/>
       <c r="C52" s="8"/>
       <c r="D52" s="9"/>
@@ -2030,7 +2030,7 @@
       <c r="I52" s="27"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="48" t="s">
+      <c r="A53" s="51" t="s">
         <v>44</v>
       </c>
       <c r="B53" s="29" t="s">
@@ -2053,7 +2053,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="49"/>
+      <c r="A54" s="52"/>
       <c r="B54" s="30" t="s">
         <v>45</v>
       </c>
@@ -2080,7 +2080,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="50"/>
+      <c r="A55" s="53"/>
       <c r="B55" s="31" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
actualizaçao de planeamento de tarefas
</commit_message>
<xml_diff>
--- a/Documentacao/planeamento de tarefas.xlsx
+++ b/Documentacao/planeamento de tarefas.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel Mendes\Desktop\TheLegend\Documentacao\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="5190"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
   <si>
     <t>Divisão de Tarefas</t>
   </si>
@@ -900,6 +895,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -949,7 +945,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,7 +965,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1008,9 +1003,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1045,7 +1040,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1080,7 +1075,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1256,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,41 +1264,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="62"/>
       <c r="H3" s="24"/>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="55" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="58"/>
-      <c r="B4" s="58"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="28" t="s">
         <v>4</v>
       </c>
@@ -1322,10 +1317,10 @@
       <c r="H4" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="55"/>
+      <c r="I4" s="56"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="49" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -1344,7 +1339,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="16" t="s">
         <v>11</v>
       </c>
@@ -1361,7 +1356,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="16" t="s">
         <v>12</v>
       </c>
@@ -1374,7 +1369,7 @@
       <c r="I7" s="26"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="16" t="s">
         <v>13</v>
       </c>
@@ -1391,7 +1386,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="16" t="s">
         <v>14</v>
       </c>
@@ -1404,7 +1399,7 @@
       <c r="I9" s="26"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="16" t="s">
         <v>15</v>
       </c>
@@ -1417,7 +1412,7 @@
       <c r="I10" s="26"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="16" t="s">
         <v>16</v>
       </c>
@@ -1430,7 +1425,7 @@
       <c r="I11" s="26"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="16" t="s">
         <v>52</v>
       </c>
@@ -1445,7 +1440,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="16" t="s">
         <v>53</v>
       </c>
@@ -1458,7 +1453,7 @@
       <c r="I13" s="26"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="16" t="s">
         <v>54</v>
       </c>
@@ -1471,7 +1466,7 @@
       <c r="I14" s="26"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="16" t="s">
         <v>17</v>
       </c>
@@ -1484,7 +1479,7 @@
       <c r="I15" s="26"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="16" t="s">
         <v>18</v>
       </c>
@@ -1497,7 +1492,7 @@
       <c r="I16" s="26"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="16" t="s">
         <v>19</v>
       </c>
@@ -1510,7 +1505,7 @@
       <c r="I17" s="26"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
+      <c r="A18" s="51"/>
       <c r="B18" s="17"/>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
@@ -1521,7 +1516,7 @@
       <c r="I18" s="27"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="49" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="15" t="s">
@@ -1529,14 +1524,18 @@
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="E19" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="12"/>
       <c r="H19" s="40"/>
-      <c r="I19" s="25"/>
+      <c r="I19" s="25" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="16" t="s">
         <v>53</v>
       </c>
@@ -1549,7 +1548,7 @@
       <c r="I20" s="26"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="16" t="s">
         <v>54</v>
       </c>
@@ -1562,7 +1561,7 @@
       <c r="I21" s="26"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="49"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="16" t="s">
         <v>20</v>
       </c>
@@ -1581,7 +1580,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="16" t="s">
         <v>21</v>
       </c>
@@ -1598,7 +1597,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="16" t="s">
         <v>22</v>
       </c>
@@ -1615,7 +1614,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="16" t="s">
         <v>23</v>
       </c>
@@ -1632,7 +1631,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="45" t="s">
         <v>64</v>
       </c>
@@ -1649,7 +1648,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="45" t="s">
         <v>65</v>
       </c>
@@ -1662,7 +1661,7 @@
       <c r="I27" s="47"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="50"/>
+      <c r="A28" s="51"/>
       <c r="B28" s="17"/>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
@@ -1673,7 +1672,7 @@
       <c r="I28" s="27"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="62" t="s">
+      <c r="A29" s="63" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="44" t="s">
@@ -1694,7 +1693,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="63"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="16" t="s">
         <v>25</v>
       </c>
@@ -1713,7 +1712,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="63"/>
+      <c r="A31" s="64"/>
       <c r="B31" s="16" t="s">
         <v>57</v>
       </c>
@@ -1732,7 +1731,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="63"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="16" t="s">
         <v>61</v>
       </c>
@@ -1751,7 +1750,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="63"/>
+      <c r="A33" s="64"/>
       <c r="B33" s="16" t="s">
         <v>63</v>
       </c>
@@ -1770,7 +1769,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="63"/>
+      <c r="A34" s="64"/>
       <c r="B34" s="16" t="s">
         <v>62</v>
       </c>
@@ -1789,7 +1788,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="63"/>
+      <c r="A35" s="64"/>
       <c r="B35" s="16" t="s">
         <v>60</v>
       </c>
@@ -1808,7 +1807,7 @@
       </c>
     </row>
     <row r="36" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="63"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="16" t="s">
         <v>59</v>
       </c>
@@ -1827,7 +1826,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="63"/>
+      <c r="A37" s="64"/>
       <c r="B37" s="16" t="s">
         <v>58</v>
       </c>
@@ -1846,7 +1845,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="63"/>
+      <c r="A38" s="64"/>
       <c r="B38" s="16" t="s">
         <v>26</v>
       </c>
@@ -1859,7 +1858,7 @@
       <c r="I38" s="26"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="63"/>
+      <c r="A39" s="64"/>
       <c r="B39" s="16" t="s">
         <v>27</v>
       </c>
@@ -1878,7 +1877,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="63"/>
+      <c r="A40" s="64"/>
       <c r="B40" s="16" t="s">
         <v>28</v>
       </c>
@@ -1891,7 +1890,7 @@
       <c r="I40" s="26"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="63"/>
+      <c r="A41" s="64"/>
       <c r="B41" s="16" t="s">
         <v>29</v>
       </c>
@@ -1908,10 +1907,10 @@
       <c r="I41" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="K41" s="65"/>
+      <c r="K41" s="48"/>
     </row>
     <row r="42" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="63"/>
+      <c r="A42" s="64"/>
       <c r="B42" s="16" t="s">
         <v>67</v>
       </c>
@@ -1930,7 +1929,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="63"/>
+      <c r="A43" s="64"/>
       <c r="B43" s="16" t="s">
         <v>66</v>
       </c>
@@ -1949,7 +1948,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="63"/>
+      <c r="A44" s="64"/>
       <c r="B44" s="16" t="s">
         <v>30</v>
       </c>
@@ -1962,7 +1961,7 @@
       <c r="I44" s="26"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="63"/>
+      <c r="A45" s="64"/>
       <c r="B45" s="16" t="s">
         <v>31</v>
       </c>
@@ -1975,7 +1974,7 @@
       <c r="I45" s="26"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="63"/>
+      <c r="A46" s="64"/>
       <c r="B46" s="16" t="s">
         <v>32</v>
       </c>
@@ -1988,7 +1987,7 @@
       <c r="I46" s="26"/>
     </row>
     <row r="47" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="63"/>
+      <c r="A47" s="64"/>
       <c r="B47" s="16" t="s">
         <v>33</v>
       </c>
@@ -2001,7 +2000,7 @@
       <c r="I47" s="26"/>
     </row>
     <row r="48" spans="1:11" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="63"/>
+      <c r="A48" s="64"/>
       <c r="B48" s="16" t="s">
         <v>68</v>
       </c>
@@ -2020,7 +2019,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="63"/>
+      <c r="A49" s="64"/>
       <c r="B49" s="16" t="s">
         <v>43</v>
       </c>
@@ -2037,7 +2036,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="64"/>
+      <c r="A50" s="65"/>
       <c r="B50" s="20"/>
       <c r="C50" s="8"/>
       <c r="D50" s="9"/>
@@ -2048,7 +2047,7 @@
       <c r="I50" s="27"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="48" t="s">
+      <c r="A51" s="49" t="s">
         <v>40</v>
       </c>
       <c r="B51" s="34" t="s">
@@ -2063,7 +2062,7 @@
       <c r="I51" s="25"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="49"/>
+      <c r="A52" s="50"/>
       <c r="B52" s="35" t="s">
         <v>35</v>
       </c>
@@ -2076,7 +2075,7 @@
       <c r="I52" s="26"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="49"/>
+      <c r="A53" s="50"/>
       <c r="B53" s="35" t="s">
         <v>36</v>
       </c>
@@ -2089,7 +2088,7 @@
       <c r="I53" s="26"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="49"/>
+      <c r="A54" s="50"/>
       <c r="B54" s="35" t="s">
         <v>37</v>
       </c>
@@ -2102,7 +2101,7 @@
       <c r="I54" s="26"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="49"/>
+      <c r="A55" s="50"/>
       <c r="B55" s="35" t="s">
         <v>38</v>
       </c>
@@ -2115,7 +2114,7 @@
       <c r="I55" s="26"/>
     </row>
     <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="50"/>
+      <c r="A56" s="51"/>
       <c r="B56" s="36"/>
       <c r="C56" s="8"/>
       <c r="D56" s="9"/>
@@ -2126,7 +2125,7 @@
       <c r="I56" s="27"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="51" t="s">
+      <c r="A57" s="52" t="s">
         <v>44</v>
       </c>
       <c r="B57" s="29" t="s">
@@ -2149,7 +2148,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="52"/>
+      <c r="A58" s="53"/>
       <c r="B58" s="30" t="s">
         <v>45</v>
       </c>
@@ -2176,7 +2175,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="53"/>
+      <c r="A59" s="54"/>
       <c r="B59" s="31" t="s">
         <v>46</v>
       </c>

</xml_diff>